<commit_message>
Excel in Python Test
</commit_message>
<xml_diff>
--- a/basic.xlsx
+++ b/basic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jibon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jibon\Coding\macroSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{168D9F29-8C11-4FE8-82DB-56CD9CD3C734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB2AF69-6C82-4358-8BAD-EDEE7C9DCD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{05F5298B-50EF-4C8D-8FDF-C76CFF9AD409}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>X</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>X*X</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C2*2</t>
   </si>
 </sst>
 </file>
@@ -395,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EF0BD1-5420-441A-8360-F6FBAAA45BCB}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,8 +419,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -425,6 +437,14 @@
       <c r="C2">
         <f>A2*A2</f>
         <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2*2</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Found a recursion problem and fixed it with cycles=True.
</commit_message>
<xml_diff>
--- a/basic.xlsx
+++ b/basic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jibon\Coding\macroSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB2AF69-6C82-4358-8BAD-EDEE7C9DCD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23188A58-39FB-4D15-9F98-4BFC37D450E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{05F5298B-50EF-4C8D-8FDF-C76CFF9AD409}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>C2*2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -401,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EF0BD1-5420-441A-8360-F6FBAAA45BCB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,6 +456,34 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <f>IF(A2=1,B4+4,C4)</f>
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(A6=1,B6,C6)</f>
+        <v>A</v>
+      </c>
+      <c r="E6">
+        <f>IF(D6="A",D4,0)</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>